<commit_message>
adjusting import mario to import mario from github repo
</commit_message>
<xml_diff>
--- a/waste-mario/Paths.xlsx
+++ b/waste-mario/Paths.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\MARIO Organization\Waste-MARIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\Waste-MARIO\DWMRIO\waste-mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBC8B18-C026-45D2-9FD7-D643B58ABF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA65F59-FEC7-4844-B291-4FF772CA94A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24468" yWindow="-108" windowWidth="24792" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>LR</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Database</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\Waste-MARIO\DWMRIO\mario</t>
+  </si>
+  <si>
+    <t>MARIO</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,25 +400,33 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update paths for LR
</commit_message>
<xml_diff>
--- a/waste-mario/Paths.xlsx
+++ b/waste-mario/Paths.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\Waste-MARIO\DWMRIO\waste-mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA65F59-FEC7-4844-B291-4FF772CA94A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970F8C04-3D5B-420A-8ECB-F630FB915430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>Add sectors non waste</t>
   </si>
   <si>
-    <t>C:\Users\loren\Documents\GitHub\MARIO Organization\Waste-MARIO\Add sectors\Add_non_waste.xlsx</t>
-  </si>
-  <si>
     <t>C:\Users\loren\OneDrive - Politecnico di Milano\Documenti\Tesi di laurea\2022-23_WasteMARIO\dMRWIO model\MARIO\Database</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>MARIO</t>
+  </si>
+  <si>
+    <t>C:\Users\loren\Documents\GitHub\Waste-MARIO\DWMRIO\waste-mario\Add sectors\Add_non_waste.xlsx</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,10 +400,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -419,15 +419,15 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creation of MRWIO (empty structure)
1. Region aggregation
2. Addition of new sectors (for new technologies and new materials)
3. Addition of waste sectors (refineries, disassembler and landfill)
4. Addition of types of waste (EoL, scraps, residues)
</commit_message>
<xml_diff>
--- a/waste-mario/Paths.xlsx
+++ b/waste-mario/Paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\DWMRIO\waste-mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055151C4-4B4F-41DD-BA7F-5AD482257DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10E78A0-5BCC-4A5C-A6F3-E8F8729D7295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-290" yWindow="1330" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>LR</t>
   </si>
@@ -42,9 +42,6 @@
     <t>CF</t>
   </si>
   <si>
-    <t>Add sectors non waste</t>
-  </si>
-  <si>
     <t>C:\Users\loren\OneDrive - Politecnico di Milano\Documenti\Tesi di laurea\2022-23_WasteMARIO\dMRWIO model\MARIO\Database</t>
   </si>
   <si>
@@ -57,12 +54,6 @@
     <t>MARIO</t>
   </si>
   <si>
-    <t>C:\Users\loren\Documents\GitHub\Waste-MARIO\DWMRIO\waste-mario\Add sectors\Add_non_waste.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\DWMRIO\waste-mario\Add sectors\Add_non_waste.xlsx</t>
-  </si>
-  <si>
     <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\IOT</t>
   </si>
   <si>
@@ -73,6 +64,27 @@
   </si>
   <si>
     <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\DWMRIO\waste-mario\Region aggregation\Region.xlsx</t>
+  </si>
+  <si>
+    <t>New sectors</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\DWMRIO\waste-mario\New sectors\New_sectors.xlsx</t>
+  </si>
+  <si>
+    <t>Waste sectors</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\DWMRIO\waste-mario\New sectors\Waste_sectors.xlsx</t>
+  </si>
+  <si>
+    <t>Type of waste</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\Desktop\UNI\MAGISTRALE\TESI\DWMRIO\waste-mario\New sectors\Type_waste.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\carol\OneDrive\Documenti\OneDrive - Politecnico di Milano\2022-23_WasteMARIO\dMRWIO model\MARIO\Database</t>
   </si>
 </sst>
 </file>
@@ -390,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -415,13 +427,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -432,34 +444,50 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>